<commit_message>
Assembly codes are running. All working. Added a instruction spreadsheet
</commit_message>
<xml_diff>
--- a/SOC_V7/SOC_V7.srcs/Instructions.xlsx
+++ b/SOC_V7/SOC_V7.srcs/Instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Vivado\Vector-Processor-SOC\SOC_V7\SOC_V7.srcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43A6E436-210A-40EF-9189-44BB02590976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6981FA93-EADF-41AC-AF74-25FE6F06642E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0506E2DF-6775-4262-A807-8FF819F8383A}"/>
   </bookViews>
@@ -352,13 +352,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -369,23 +366,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -397,25 +396,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -906,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55F3AF4-C273-46A4-AD79-C2CE4FB3B1BC}">
   <dimension ref="C7:AP38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="AP18" sqref="AP18"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -921,217 +917,193 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="2"/>
-      <c r="AL7" s="2"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="17"/>
+      <c r="AF7" s="17"/>
+      <c r="AG7" s="17"/>
+      <c r="AH7" s="17"/>
+      <c r="AI7" s="17"/>
+      <c r="AJ7" s="17"/>
+      <c r="AK7" s="17"/>
+      <c r="AL7" s="17"/>
     </row>
     <row r="8" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
-      <c r="AF8" s="6"/>
-      <c r="AG8" s="6"/>
-      <c r="AH8" s="6"/>
-      <c r="AI8" s="6"/>
-      <c r="AJ8" s="6"/>
-      <c r="AK8" s="6"/>
-      <c r="AL8" s="6"/>
+      <c r="G8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
     </row>
     <row r="9" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>31</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>30</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>29</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>28</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>27</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>26</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>25</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>24</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="2">
         <v>23</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="2">
         <v>22</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9" s="2">
         <v>21</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="2">
         <v>20</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="2">
         <v>19</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="2">
         <v>18</v>
       </c>
-      <c r="U9" s="3">
+      <c r="U9" s="2">
         <v>17</v>
       </c>
-      <c r="V9" s="3">
+      <c r="V9" s="2">
         <v>16</v>
       </c>
-      <c r="W9" s="3">
+      <c r="W9" s="2">
         <v>15</v>
       </c>
-      <c r="X9" s="3">
+      <c r="X9" s="2">
         <v>14</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="Y9" s="2">
         <v>13</v>
       </c>
-      <c r="Z9" s="3">
+      <c r="Z9" s="2">
         <v>12</v>
       </c>
-      <c r="AA9" s="3">
+      <c r="AA9" s="2">
         <v>11</v>
       </c>
-      <c r="AB9" s="3">
+      <c r="AB9" s="2">
         <v>10</v>
       </c>
-      <c r="AC9" s="3">
+      <c r="AC9" s="2">
         <v>9</v>
       </c>
-      <c r="AD9" s="3">
+      <c r="AD9" s="2">
         <v>8</v>
       </c>
-      <c r="AE9" s="3">
+      <c r="AE9" s="2">
         <v>7</v>
       </c>
-      <c r="AF9" s="3">
+      <c r="AF9" s="2">
         <v>6</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AG9" s="2">
         <v>5</v>
       </c>
-      <c r="AH9" s="3">
+      <c r="AH9" s="2">
         <v>4</v>
       </c>
-      <c r="AI9" s="3">
+      <c r="AI9" s="2">
         <v>3</v>
       </c>
-      <c r="AJ9" s="3">
+      <c r="AJ9" s="2">
         <v>2</v>
       </c>
-      <c r="AK9" s="3">
+      <c r="AK9" s="2">
         <v>1</v>
       </c>
-      <c r="AL9" s="3">
+      <c r="AL9" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="4"/>
-      <c r="AB10" s="4"/>
-      <c r="AC10" s="4"/>
-      <c r="AD10" s="4"/>
-      <c r="AE10" s="4"/>
-      <c r="AF10" s="4"/>
-      <c r="AG10" s="4"/>
-      <c r="AH10" s="4"/>
-      <c r="AI10" s="4"/>
-      <c r="AJ10" s="4"/>
-      <c r="AK10" s="4"/>
-      <c r="AL10" s="4"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
     </row>
     <row r="11" spans="3:42" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
@@ -1143,100 +1115,100 @@
       <c r="E11" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5">
-        <v>0</v>
-      </c>
-      <c r="M11" s="5">
-        <v>0</v>
-      </c>
-      <c r="N11" s="5">
-        <v>0</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AK11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL11" s="4" t="s">
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL11" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1250,136 +1222,136 @@
       <c r="E12" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
-        <v>0</v>
-      </c>
-      <c r="L12" s="5">
-        <v>0</v>
-      </c>
-      <c r="M12" s="5">
-        <v>0</v>
-      </c>
-      <c r="N12" s="5">
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
         <v>1</v>
       </c>
-      <c r="O12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="S12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="U12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="V12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AK12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL12" s="4" t="s">
+      <c r="O12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL12" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="4"/>
-      <c r="AF13" s="4"/>
-      <c r="AG13" s="4"/>
-      <c r="AH13" s="4"/>
-      <c r="AI13" s="4"/>
-      <c r="AJ13" s="4"/>
-      <c r="AK13" s="4"/>
-      <c r="AL13" s="4"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
     </row>
     <row r="14" spans="3:42" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
@@ -1391,56 +1363,56 @@
       <c r="E14" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="5">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-      <c r="K14" s="5">
-        <v>0</v>
-      </c>
-      <c r="L14" s="5">
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
         <v>1</v>
       </c>
-      <c r="M14" s="5">
-        <v>0</v>
-      </c>
-      <c r="N14" s="5">
-        <v>0</v>
-      </c>
-      <c r="O14" s="8" t="s">
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
-      <c r="AI14" s="9"/>
-      <c r="AJ14" s="9"/>
-      <c r="AK14" s="9"/>
-      <c r="AL14" s="10"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19"/>
+      <c r="AG14" s="19"/>
+      <c r="AH14" s="19"/>
+      <c r="AI14" s="19"/>
+      <c r="AJ14" s="19"/>
+      <c r="AK14" s="19"/>
+      <c r="AL14" s="20"/>
     </row>
     <row r="15" spans="3:42" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
@@ -1452,97 +1424,97 @@
       <c r="E15" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <v>0</v>
-      </c>
-      <c r="K15" s="5">
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
         <v>1</v>
       </c>
-      <c r="L15" s="5">
-        <v>0</v>
-      </c>
-      <c r="M15" s="5">
-        <v>0</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0</v>
-      </c>
-      <c r="O15" s="8" t="s">
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="9"/>
-      <c r="AF15" s="9"/>
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="9"/>
-      <c r="AI15" s="9"/>
-      <c r="AJ15" s="9"/>
-      <c r="AK15" s="9"/>
-      <c r="AL15" s="10"/>
-      <c r="AN15" s="22" t="s">
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19"/>
+      <c r="AG15" s="19"/>
+      <c r="AH15" s="19"/>
+      <c r="AI15" s="19"/>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="19"/>
+      <c r="AL15" s="20"/>
+      <c r="AN15" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="AO15" s="22"/>
-      <c r="AP15" s="11" t="s">
+      <c r="AO15" s="15"/>
+      <c r="AP15" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="4"/>
-      <c r="AC16" s="4"/>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="4"/>
-      <c r="AF16" s="4"/>
-      <c r="AG16" s="4"/>
-      <c r="AH16" s="4"/>
-      <c r="AI16" s="4"/>
-      <c r="AJ16" s="4"/>
-      <c r="AK16" s="4"/>
-      <c r="AL16" s="4"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3"/>
+      <c r="AL16" s="3"/>
       <c r="AN16" s="1">
         <v>0</v>
       </c>
@@ -1563,62 +1535,62 @@
       <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5">
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
         <v>1</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="4">
         <v>1</v>
       </c>
-      <c r="M17" s="5">
-        <v>0</v>
-      </c>
-      <c r="N17" s="5">
-        <v>0</v>
-      </c>
-      <c r="O17" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="P17" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q17" s="16" t="s">
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
-      <c r="W17" s="17"/>
-      <c r="X17" s="17"/>
-      <c r="Y17" s="17"/>
-      <c r="Z17" s="17"/>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="13" t="s">
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="14"/>
-      <c r="AE17" s="14"/>
-      <c r="AF17" s="14"/>
-      <c r="AG17" s="14"/>
-      <c r="AH17" s="14"/>
-      <c r="AI17" s="14"/>
-      <c r="AJ17" s="14"/>
-      <c r="AK17" s="14"/>
-      <c r="AL17" s="15"/>
+      <c r="AC17" s="13"/>
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="13"/>
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="13"/>
+      <c r="AH17" s="13"/>
+      <c r="AI17" s="13"/>
+      <c r="AJ17" s="13"/>
+      <c r="AK17" s="13"/>
+      <c r="AL17" s="14"/>
       <c r="AN17" s="1">
         <v>0</v>
       </c>
@@ -1639,60 +1611,60 @@
       <c r="E18" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0</v>
-      </c>
-      <c r="K18" s="5">
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
         <v>1</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="4">
         <v>1</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="4">
         <v>1</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="4">
         <v>1</v>
       </c>
-      <c r="O18" s="19" t="s">
+      <c r="O18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="16" t="s">
+      <c r="P18" s="8"/>
+      <c r="Q18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="17"/>
-      <c r="V18" s="17"/>
-      <c r="W18" s="17"/>
-      <c r="X18" s="17"/>
-      <c r="Y18" s="17"/>
-      <c r="Z18" s="17"/>
-      <c r="AA18" s="18"/>
-      <c r="AB18" s="13" t="s">
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AC18" s="14"/>
-      <c r="AD18" s="14"/>
-      <c r="AE18" s="14"/>
-      <c r="AF18" s="14"/>
-      <c r="AG18" s="14"/>
-      <c r="AH18" s="14"/>
-      <c r="AI18" s="14"/>
-      <c r="AJ18" s="14"/>
-      <c r="AK18" s="14"/>
-      <c r="AL18" s="15"/>
+      <c r="AC18" s="13"/>
+      <c r="AD18" s="13"/>
+      <c r="AE18" s="13"/>
+      <c r="AF18" s="13"/>
+      <c r="AG18" s="13"/>
+      <c r="AH18" s="13"/>
+      <c r="AI18" s="13"/>
+      <c r="AJ18" s="13"/>
+      <c r="AK18" s="13"/>
+      <c r="AL18" s="14"/>
       <c r="AN18" s="1">
         <v>1</v>
       </c>
@@ -1704,38 +1676,38 @@
       </c>
     </row>
     <row r="19" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="4"/>
-      <c r="AB19" s="4"/>
-      <c r="AC19" s="4"/>
-      <c r="AD19" s="4"/>
-      <c r="AE19" s="4"/>
-      <c r="AF19" s="4"/>
-      <c r="AG19" s="4"/>
-      <c r="AH19" s="4"/>
-      <c r="AI19" s="4"/>
-      <c r="AJ19" s="4"/>
-      <c r="AK19" s="4"/>
-      <c r="AL19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="3"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3"/>
+      <c r="AK19" s="3"/>
+      <c r="AL19" s="3"/>
       <c r="AN19" s="1">
         <v>1</v>
       </c>
@@ -1747,242 +1719,242 @@
       </c>
     </row>
     <row r="20" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
-      <c r="AC20" s="4"/>
-      <c r="AD20" s="4"/>
-      <c r="AE20" s="4"/>
-      <c r="AF20" s="4"/>
-      <c r="AG20" s="4"/>
-      <c r="AH20" s="4"/>
-      <c r="AI20" s="4"/>
-      <c r="AJ20" s="4"/>
-      <c r="AK20" s="4"/>
-      <c r="AL20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="3"/>
     </row>
     <row r="21" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="4"/>
-      <c r="AC21" s="4"/>
-      <c r="AD21" s="4"/>
-      <c r="AE21" s="4"/>
-      <c r="AF21" s="4"/>
-      <c r="AG21" s="4"/>
-      <c r="AH21" s="4"/>
-      <c r="AI21" s="4"/>
-      <c r="AJ21" s="4"/>
-      <c r="AK21" s="4"/>
-      <c r="AL21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3"/>
+      <c r="AG21" s="3"/>
+      <c r="AH21" s="3"/>
+      <c r="AI21" s="3"/>
+      <c r="AJ21" s="3"/>
+      <c r="AK21" s="3"/>
+      <c r="AL21" s="3"/>
     </row>
     <row r="22" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
-      <c r="AB22" s="4"/>
-      <c r="AC22" s="4"/>
-      <c r="AD22" s="4"/>
-      <c r="AE22" s="4"/>
-      <c r="AF22" s="4"/>
-      <c r="AG22" s="4"/>
-      <c r="AH22" s="4"/>
-      <c r="AI22" s="4"/>
-      <c r="AJ22" s="4"/>
-      <c r="AK22" s="4"/>
-      <c r="AL22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
     </row>
     <row r="23" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
-      <c r="AA23" s="4"/>
-      <c r="AB23" s="4"/>
-      <c r="AC23" s="4"/>
-      <c r="AD23" s="4"/>
-      <c r="AE23" s="4"/>
-      <c r="AF23" s="4"/>
-      <c r="AG23" s="4"/>
-      <c r="AH23" s="4"/>
-      <c r="AI23" s="4"/>
-      <c r="AJ23" s="4"/>
-      <c r="AK23" s="4"/>
-      <c r="AL23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
     </row>
     <row r="24" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-      <c r="Z24" s="4"/>
-      <c r="AA24" s="4"/>
-      <c r="AB24" s="4"/>
-      <c r="AC24" s="4"/>
-      <c r="AD24" s="4"/>
-      <c r="AE24" s="4"/>
-      <c r="AF24" s="4"/>
-      <c r="AG24" s="4"/>
-      <c r="AH24" s="4"/>
-      <c r="AI24" s="4"/>
-      <c r="AJ24" s="4"/>
-      <c r="AK24" s="4"/>
-      <c r="AL24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
     </row>
     <row r="25" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
-      <c r="AB25" s="4"/>
-      <c r="AC25" s="4"/>
-      <c r="AD25" s="4"/>
-      <c r="AE25" s="4"/>
-      <c r="AF25" s="4"/>
-      <c r="AG25" s="4"/>
-      <c r="AH25" s="4"/>
-      <c r="AI25" s="4"/>
-      <c r="AJ25" s="4"/>
-      <c r="AK25" s="4"/>
-      <c r="AL25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
     </row>
     <row r="26" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="4"/>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="4"/>
-      <c r="AD26" s="4"/>
-      <c r="AE26" s="4"/>
-      <c r="AF26" s="4"/>
-      <c r="AG26" s="4"/>
-      <c r="AH26" s="4"/>
-      <c r="AI26" s="4"/>
-      <c r="AJ26" s="4"/>
-      <c r="AK26" s="4"/>
-      <c r="AL26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
     </row>
     <row r="27" spans="3:42" x14ac:dyDescent="0.3">
       <c r="G27" s="1"/>
@@ -2394,16 +2366,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G7:AL7"/>
+    <mergeCell ref="O14:AL14"/>
+    <mergeCell ref="O15:AL15"/>
+    <mergeCell ref="AB17:AL17"/>
+    <mergeCell ref="Q17:AA17"/>
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="Q18:AA18"/>
     <mergeCell ref="AB18:AL18"/>
     <mergeCell ref="AN15:AO15"/>
     <mergeCell ref="G8:N8"/>
-    <mergeCell ref="G7:AL7"/>
-    <mergeCell ref="O14:AL14"/>
-    <mergeCell ref="O15:AL15"/>
-    <mergeCell ref="AB17:AL17"/>
-    <mergeCell ref="Q17:AA17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New PE created tested and working all.
</commit_message>
<xml_diff>
--- a/SOC_V7/SOC_V7.srcs/Instructions.xlsx
+++ b/SOC_V7/SOC_V7.srcs/Instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Vivado\Vector-Processor-SOC\SOC_V7\SOC_V7.srcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6981FA93-EADF-41AC-AF74-25FE6F06642E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A87D1BB-5686-4A43-A5FE-23D58D8624F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0506E2DF-6775-4262-A807-8FF819F8383A}"/>
   </bookViews>
@@ -228,6 +228,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -256,12 +257,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -275,6 +270,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -357,9 +358,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -369,22 +367,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -396,22 +397,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -903,7 +904,7 @@
   <dimension ref="C7:AP38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="AP29" sqref="AP29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,193 +918,193 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="17"/>
-      <c r="AB7" s="17"/>
-      <c r="AC7" s="17"/>
-      <c r="AD7" s="17"/>
-      <c r="AE7" s="17"/>
-      <c r="AF7" s="17"/>
-      <c r="AG7" s="17"/>
-      <c r="AH7" s="17"/>
-      <c r="AI7" s="17"/>
-      <c r="AJ7" s="17"/>
-      <c r="AK7" s="17"/>
-      <c r="AL7" s="17"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
     </row>
     <row r="8" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G8" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
+      <c r="G8" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
     </row>
     <row r="9" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="19">
         <v>31</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="19">
         <v>30</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="19">
         <v>29</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="19">
         <v>28</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="19">
         <v>27</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="19">
         <v>26</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="19">
         <v>25</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="19">
         <v>24</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="19">
         <v>23</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="19">
         <v>22</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="19">
         <v>21</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="19">
         <v>20</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9" s="19">
         <v>19</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="19">
         <v>18</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9" s="19">
         <v>17</v>
       </c>
-      <c r="V9" s="2">
+      <c r="V9" s="19">
         <v>16</v>
       </c>
-      <c r="W9" s="2">
+      <c r="W9" s="19">
         <v>15</v>
       </c>
-      <c r="X9" s="2">
+      <c r="X9" s="19">
         <v>14</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Y9" s="19">
         <v>13</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="Z9" s="19">
         <v>12</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AA9" s="19">
         <v>11</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AB9" s="19">
         <v>10</v>
       </c>
-      <c r="AC9" s="2">
+      <c r="AC9" s="19">
         <v>9</v>
       </c>
-      <c r="AD9" s="2">
+      <c r="AD9" s="19">
         <v>8</v>
       </c>
-      <c r="AE9" s="2">
+      <c r="AE9" s="19">
         <v>7</v>
       </c>
-      <c r="AF9" s="2">
+      <c r="AF9" s="19">
         <v>6</v>
       </c>
-      <c r="AG9" s="2">
+      <c r="AG9" s="19">
         <v>5</v>
       </c>
-      <c r="AH9" s="2">
+      <c r="AH9" s="19">
         <v>4</v>
       </c>
-      <c r="AI9" s="2">
+      <c r="AI9" s="19">
         <v>3</v>
       </c>
-      <c r="AJ9" s="2">
+      <c r="AJ9" s="19">
         <v>2</v>
       </c>
-      <c r="AK9" s="2">
+      <c r="AK9" s="19">
         <v>1</v>
       </c>
-      <c r="AL9" s="2">
+      <c r="AL9" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
-      <c r="AJ10" s="3"/>
-      <c r="AK10" s="3"/>
-      <c r="AL10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
     </row>
     <row r="11" spans="3:42" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
@@ -1115,100 +1116,100 @@
       <c r="E11" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="4">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
-        <v>0</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0</v>
-      </c>
-      <c r="N11" s="4">
-        <v>0</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AK11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL11" s="3" t="s">
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="S11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="T11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="U11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="W11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="X11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL11" s="20" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1222,136 +1223,136 @@
       <c r="E12" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="4">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
-        <v>0</v>
-      </c>
-      <c r="K12" s="4">
-        <v>0</v>
-      </c>
-      <c r="L12" s="4">
-        <v>0</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0</v>
-      </c>
-      <c r="N12" s="4">
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
         <v>1</v>
       </c>
-      <c r="O12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="X12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AK12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL12" s="3" t="s">
+      <c r="O12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="R12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="S12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="T12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="U12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="V12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="W12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="X12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL12" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
-      <c r="AD13" s="3"/>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="3"/>
-      <c r="AG13" s="3"/>
-      <c r="AH13" s="3"/>
-      <c r="AI13" s="3"/>
-      <c r="AJ13" s="3"/>
-      <c r="AK13" s="3"/>
-      <c r="AL13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
     </row>
     <row r="14" spans="3:42" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
@@ -1363,56 +1364,56 @@
       <c r="E14" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="4">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
         <v>1</v>
       </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
-      <c r="N14" s="4">
-        <v>0</v>
-      </c>
-      <c r="O14" s="18" t="s">
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0</v>
+      </c>
+      <c r="O14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
-      <c r="V14" s="19"/>
-      <c r="W14" s="19"/>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="19"/>
-      <c r="AA14" s="19"/>
-      <c r="AB14" s="19"/>
-      <c r="AC14" s="19"/>
-      <c r="AD14" s="19"/>
-      <c r="AE14" s="19"/>
-      <c r="AF14" s="19"/>
-      <c r="AG14" s="19"/>
-      <c r="AH14" s="19"/>
-      <c r="AI14" s="19"/>
-      <c r="AJ14" s="19"/>
-      <c r="AK14" s="19"/>
-      <c r="AL14" s="20"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="7"/>
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="7"/>
+      <c r="AL14" s="8"/>
     </row>
     <row r="15" spans="3:42" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
@@ -1424,97 +1425,97 @@
       <c r="E15" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
         <v>1</v>
       </c>
-      <c r="L15" s="4">
-        <v>0</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0</v>
-      </c>
-      <c r="N15" s="4">
-        <v>0</v>
-      </c>
-      <c r="O15" s="18" t="s">
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19"/>
-      <c r="AA15" s="19"/>
-      <c r="AB15" s="19"/>
-      <c r="AC15" s="19"/>
-      <c r="AD15" s="19"/>
-      <c r="AE15" s="19"/>
-      <c r="AF15" s="19"/>
-      <c r="AG15" s="19"/>
-      <c r="AH15" s="19"/>
-      <c r="AI15" s="19"/>
-      <c r="AJ15" s="19"/>
-      <c r="AK15" s="19"/>
-      <c r="AL15" s="20"/>
-      <c r="AN15" s="15" t="s">
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7"/>
+      <c r="AL15" s="8"/>
+      <c r="AN15" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="AO15" s="15"/>
-      <c r="AP15" s="5" t="s">
+      <c r="AO15" s="17"/>
+      <c r="AP15" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="3"/>
-      <c r="AD16" s="3"/>
-      <c r="AE16" s="3"/>
-      <c r="AF16" s="3"/>
-      <c r="AG16" s="3"/>
-      <c r="AH16" s="3"/>
-      <c r="AI16" s="3"/>
-      <c r="AJ16" s="3"/>
-      <c r="AK16" s="3"/>
-      <c r="AL16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
       <c r="AN16" s="1">
         <v>0</v>
       </c>
@@ -1535,62 +1536,62 @@
       <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
-        <v>0</v>
-      </c>
-      <c r="K17" s="4">
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
         <v>1</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="3">
         <v>1</v>
       </c>
-      <c r="M17" s="4">
-        <v>0</v>
-      </c>
-      <c r="N17" s="4">
-        <v>0</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q17" s="9" t="s">
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0</v>
+      </c>
+      <c r="O17" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q17" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="12" t="s">
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="14"/>
+      <c r="AB17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="13"/>
-      <c r="AE17" s="13"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="13"/>
-      <c r="AI17" s="13"/>
-      <c r="AJ17" s="13"/>
-      <c r="AK17" s="13"/>
-      <c r="AL17" s="14"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="10"/>
+      <c r="AE17" s="10"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="10"/>
+      <c r="AJ17" s="10"/>
+      <c r="AK17" s="10"/>
+      <c r="AL17" s="11"/>
       <c r="AN17" s="1">
         <v>0</v>
       </c>
@@ -1611,60 +1612,60 @@
       <c r="E18" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
         <v>1</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="3">
         <v>1</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="3">
         <v>1</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18" s="3">
         <v>1</v>
       </c>
-      <c r="O18" s="7" t="s">
+      <c r="O18" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="9" t="s">
+      <c r="P18" s="16"/>
+      <c r="Q18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="12" t="s">
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AC18" s="13"/>
-      <c r="AD18" s="13"/>
-      <c r="AE18" s="13"/>
-      <c r="AF18" s="13"/>
-      <c r="AG18" s="13"/>
-      <c r="AH18" s="13"/>
-      <c r="AI18" s="13"/>
-      <c r="AJ18" s="13"/>
-      <c r="AK18" s="13"/>
-      <c r="AL18" s="14"/>
+      <c r="AC18" s="10"/>
+      <c r="AD18" s="10"/>
+      <c r="AE18" s="10"/>
+      <c r="AF18" s="10"/>
+      <c r="AG18" s="10"/>
+      <c r="AH18" s="10"/>
+      <c r="AI18" s="10"/>
+      <c r="AJ18" s="10"/>
+      <c r="AK18" s="10"/>
+      <c r="AL18" s="11"/>
       <c r="AN18" s="1">
         <v>1</v>
       </c>
@@ -1676,38 +1677,38 @@
       </c>
     </row>
     <row r="19" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
-      <c r="AF19" s="3"/>
-      <c r="AG19" s="3"/>
-      <c r="AH19" s="3"/>
-      <c r="AI19" s="3"/>
-      <c r="AJ19" s="3"/>
-      <c r="AK19" s="3"/>
-      <c r="AL19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="2"/>
+      <c r="AK19" s="2"/>
+      <c r="AL19" s="2"/>
       <c r="AN19" s="1">
         <v>1</v>
       </c>
@@ -1719,242 +1720,242 @@
       </c>
     </row>
     <row r="20" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="3"/>
-      <c r="AG20" s="3"/>
-      <c r="AH20" s="3"/>
-      <c r="AI20" s="3"/>
-      <c r="AJ20" s="3"/>
-      <c r="AK20" s="3"/>
-      <c r="AL20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AJ20" s="2"/>
+      <c r="AK20" s="2"/>
+      <c r="AL20" s="2"/>
     </row>
     <row r="21" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
-      <c r="AF21" s="3"/>
-      <c r="AG21" s="3"/>
-      <c r="AH21" s="3"/>
-      <c r="AI21" s="3"/>
-      <c r="AJ21" s="3"/>
-      <c r="AK21" s="3"/>
-      <c r="AL21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
     </row>
     <row r="22" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
-      <c r="AE22" s="3"/>
-      <c r="AF22" s="3"/>
-      <c r="AG22" s="3"/>
-      <c r="AH22" s="3"/>
-      <c r="AI22" s="3"/>
-      <c r="AJ22" s="3"/>
-      <c r="AK22" s="3"/>
-      <c r="AL22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
     </row>
     <row r="23" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="3"/>
-      <c r="AD23" s="3"/>
-      <c r="AE23" s="3"/>
-      <c r="AF23" s="3"/>
-      <c r="AG23" s="3"/>
-      <c r="AH23" s="3"/>
-      <c r="AI23" s="3"/>
-      <c r="AJ23" s="3"/>
-      <c r="AK23" s="3"/>
-      <c r="AL23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="2"/>
     </row>
     <row r="24" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
-      <c r="AA24" s="3"/>
-      <c r="AB24" s="3"/>
-      <c r="AC24" s="3"/>
-      <c r="AD24" s="3"/>
-      <c r="AE24" s="3"/>
-      <c r="AF24" s="3"/>
-      <c r="AG24" s="3"/>
-      <c r="AH24" s="3"/>
-      <c r="AI24" s="3"/>
-      <c r="AJ24" s="3"/>
-      <c r="AK24" s="3"/>
-      <c r="AL24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="2"/>
+      <c r="AL24" s="2"/>
     </row>
     <row r="25" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
-      <c r="AA25" s="3"/>
-      <c r="AB25" s="3"/>
-      <c r="AC25" s="3"/>
-      <c r="AD25" s="3"/>
-      <c r="AE25" s="3"/>
-      <c r="AF25" s="3"/>
-      <c r="AG25" s="3"/>
-      <c r="AH25" s="3"/>
-      <c r="AI25" s="3"/>
-      <c r="AJ25" s="3"/>
-      <c r="AK25" s="3"/>
-      <c r="AL25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
     </row>
     <row r="26" spans="3:42" x14ac:dyDescent="0.3">
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
-      <c r="AA26" s="3"/>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="3"/>
-      <c r="AD26" s="3"/>
-      <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="3"/>
-      <c r="AH26" s="3"/>
-      <c r="AI26" s="3"/>
-      <c r="AJ26" s="3"/>
-      <c r="AK26" s="3"/>
-      <c r="AL26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="2"/>
+      <c r="AL26" s="2"/>
     </row>
     <row r="27" spans="3:42" x14ac:dyDescent="0.3">
       <c r="G27" s="1"/>
@@ -2366,16 +2367,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:AA18"/>
+    <mergeCell ref="AB18:AL18"/>
+    <mergeCell ref="AN15:AO15"/>
+    <mergeCell ref="G8:N8"/>
     <mergeCell ref="G7:AL7"/>
     <mergeCell ref="O14:AL14"/>
     <mergeCell ref="O15:AL15"/>
     <mergeCell ref="AB17:AL17"/>
     <mergeCell ref="Q17:AA17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:AA18"/>
-    <mergeCell ref="AB18:AL18"/>
-    <mergeCell ref="AN15:AO15"/>
-    <mergeCell ref="G8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>